<commit_message>
Edit of the CSV version of the metajelo schema.
</commit_message>
<xml_diff>
--- a/schema/tabular-metajelo.xlsx
+++ b/schema/tabular-metajelo.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="103">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -49,7 +49,7 @@
     <t xml:space="preserve">identifier</t>
   </si>
   <si>
-    <t xml:space="preserve">Persistent id (e.g., DOI) assigned to this metadata record</t>
+    <t xml:space="preserve">Persistent ID assigned to this metajelo record (ID types attribute: DataCite) </t>
   </si>
   <si>
     <t xml:space="preserve">date</t>
@@ -67,13 +67,13 @@
     <t xml:space="preserve">relatedIdentifier</t>
   </si>
   <si>
-    <t xml:space="preserve">Identifiers (links) to the object with which the supplementary products are associated.  This could be a link to the object itself or to metadata, etc.  Note presence of attribute indicating relationship type.  Note also controlled vocabular of relation types.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Repeatable, </t>
-  </si>
-  <si>
-    <t xml:space="preserve">relationship ID types and relationship types are copied from DataCite</t>
+    <t xml:space="preserve">Identifiers (links) to the object (article) with which the supplementary products are associated (ID types attribute: DataCite)  This could be a link to the object itself or to metadata.  Note presence of attribute indicating relationship type, controlled vocabular of datacite:relationTypes .</t>
+  </si>
+  <si>
+    <t xml:space="preserve">repeatable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DataCite</t>
   </si>
   <si>
     <t xml:space="preserve">supplementaryProducts</t>
@@ -92,16 +92,13 @@
     <t xml:space="preserve">Wrapper element around the metadata for an individual supplementary product.</t>
   </si>
   <si>
-    <t xml:space="preserve">repeatable</t>
-  </si>
-  <si>
     <t xml:space="preserve">1.5.1.1 </t>
   </si>
   <si>
-    <t xml:space="preserve">productID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Persistent ID (ARK, DOI, UUID, etc.) of supplementary product</t>
+    <t xml:space="preserve">resourceID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Persistent ID  of supplementary product  (ID types attribute: DataCite) </t>
   </si>
   <si>
     <t xml:space="preserve">Optional (some products will not have PID)</t>
@@ -116,25 +113,31 @@
     <t xml:space="preserve">basicMetadata</t>
   </si>
   <si>
-    <t xml:space="preserve">Simple bibliographic metadata</t>
+    <t xml:space="preserve">Bibliographic metadata (Creator, Title, PublicationYear [DataCite]). Note that Publisher is drawn from institutionName.</t>
   </si>
   <si>
     <t xml:space="preserve">Required</t>
   </si>
   <si>
-    <t xml:space="preserve">DataCite</t>
-  </si>
-  <si>
     <t xml:space="preserve">Copy from DataCite</t>
   </si>
   <si>
     <t xml:space="preserve">1.5.1.2</t>
   </si>
   <si>
-    <t xml:space="preserve">productType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Genre of supplementary product</t>
+    <t xml:space="preserve">resourceType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description of supplementary product</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.5.1.2.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">resourceTypeGeneral</t>
+  </si>
+  <si>
+    <t xml:space="preserve">General type of the supplementary product. </t>
   </si>
   <si>
     <t xml:space="preserve">Controlled vocabulary </t>
@@ -143,10 +146,10 @@
     <t xml:space="preserve">1.5.1.3</t>
   </si>
   <si>
-    <t xml:space="preserve">formats</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Technical format of the product (e.g., stata, csv, zip, gzip)</t>
+    <t xml:space="preserve">Format</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Technical format of the product (e.g., stata, csv, zip, gzip). Use file extension or MIME type if possible.</t>
   </si>
   <si>
     <t xml:space="preserve">optional, repeatable</t>
@@ -155,10 +158,10 @@
     <t xml:space="preserve">1.5.1.4</t>
   </si>
   <si>
-    <t xml:space="preserve">productMetadataSource</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Handle referencing metadata describing this supplementary product (e.g., in DataCIte)</t>
+    <t xml:space="preserve">resourceMetadataSource</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Handle referencing metadata describing this supplementary product (e.g., in DataCite) (ID types attribute: DataCite) </t>
   </si>
   <si>
     <t xml:space="preserve">optional</t>
@@ -179,24 +182,30 @@
     <t xml:space="preserve">institutionID</t>
   </si>
   <si>
-    <t xml:space="preserve">Persistent identifier (DOI, ARK, etc.) of location (repository, archive, etc.)</t>
+    <t xml:space="preserve">Persistent ID assigned to the institution holding this object  (ID types attribute: DataCite). This should be the same as in re3data, CoreTrustSeal, etc.</t>
   </si>
   <si>
     <t xml:space="preserve">re3data</t>
   </si>
   <si>
+    <t xml:space="preserve">Should this be repeatable? If we have a re3data, a FunderRef, and an OpenAIRE ID?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.5.1.5.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">institutionName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Free text name of location. Maps to datacite:Publisher and re3data:repositoryName or re3data:institutionName. Used for bibliographic citation.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">re3data, DataCite</t>
+  </si>
+  <si>
     <t xml:space="preserve">This should be consistent with re3data schema</t>
   </si>
   <si>
-    <t xml:space="preserve">1.5.1.5.2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">institutionName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Free text name of location.</t>
-  </si>
-  <si>
     <t xml:space="preserve">1.5.1.5.3</t>
   </si>
   <si>
@@ -206,7 +215,7 @@
     <t xml:space="preserve">Organization type of the location.</t>
   </si>
   <si>
-    <t xml:space="preserve">Controlled vocabulary – commercial, non-profit, governmental (will be expanded in future),</t>
+    <t xml:space="preserve">Controlled vocabulary based on re3data, possibly expanded</t>
   </si>
   <si>
     <t xml:space="preserve">1.5.1.5.4</t>
@@ -227,7 +236,10 @@
     <t xml:space="preserve">institutionContact</t>
   </si>
   <si>
-    <t xml:space="preserve">Email address of contact party</t>
+    <t xml:space="preserve">Email address or online contact form of contact party</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Suggested</t>
   </si>
   <si>
     <t xml:space="preserve">1.5.1.5.6</t>
@@ -272,28 +284,40 @@
     <t xml:space="preserve">institutionPolicy</t>
   </si>
   <si>
-    <t xml:space="preserve">A policy of the institution; attribute policyType specifies the nature of the policy (access, collection, etc.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Repeatable.  Attribute appliesToProduct is true for policies that apply to this product.</t>
+    <t xml:space="preserve">A policy of the institution.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Repeatable.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Attribute re3data:policyType specifies the nature of the policy (access, collection, etc.). We also include License here.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">At least one of Preservation policy and (Terms of Use or License) are required.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Attribute appliesToProduct is true for policies that apply to this product. </t>
   </si>
   <si>
     <t xml:space="preserve">1.5.1.5.7.1.1</t>
   </si>
   <si>
-    <t xml:space="preserve">freeTextPolicy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A free text explanation of the policy</t>
+    <t xml:space="preserve">institutionPolicyFreeText</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A free text explanation of the policy. This may be scraped from the URI if not a PID.</t>
   </si>
   <si>
     <t xml:space="preserve">Choice</t>
   </si>
   <si>
-    <t xml:space="preserve">refPolicy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">URI of policy</t>
+    <t xml:space="preserve">1.5.1.5.7.1.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">institutionPolicyURL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">URI of policy. Attribute re3data:policyURL points to an online copy of the policy. (ID types attribute: DataCite) </t>
   </si>
   <si>
     <t xml:space="preserve">1.5.1.5.7.2</t>
@@ -302,7 +326,10 @@
     <t xml:space="preserve">versioning</t>
   </si>
   <si>
-    <t xml:space="preserve">Yes or no, does the location support versioning of content</t>
+    <t xml:space="preserve">Does the location support versioning of content</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Allowed values: yes, no, unknown</t>
   </si>
 </sst>
 </file>
@@ -317,6 +344,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -337,18 +365,21 @@
       <sz val="12"/>
       <name val="Calibri"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFCE181E"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FFCE181E"/>
       <name val="Calibri"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -487,12 +518,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -562,16 +593,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A18" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E23" activeCellId="0" sqref="E23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="23.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="23.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="36.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="28.34"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="11.52"/>
@@ -610,7 +641,7 @@
       </c>
       <c r="D2" s="5"/>
     </row>
-    <row r="3" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="27.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="n">
         <v>1.1</v>
       </c>
@@ -646,7 +677,7 @@
       </c>
       <c r="D5" s="5"/>
     </row>
-    <row r="6" customFormat="false" ht="97" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="105.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="n">
         <v>1.4</v>
       </c>
@@ -686,186 +717,194 @@
         <v>22</v>
       </c>
       <c r="D8" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="27.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="4" t="s">
+      <c r="B9" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="C9" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="D9" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="F9" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="F9" s="10" t="s">
+    </row>
+    <row r="10" customFormat="false" ht="40.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="11" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="11" t="s">
+      <c r="B10" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="C10" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="D10" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="E10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="14" t="s">
         <v>32</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F10" s="14" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="D11" s="0"/>
+      <c r="E11" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="27.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="B12" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="C12" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E11" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="4" t="s">
+      <c r="D12" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="E12" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="40.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="B13" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="C13" s="5" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="13" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="4" t="s">
+      <c r="D13" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="E13" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="40.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="B14" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="C14" s="5" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="14" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="4" t="s">
+      <c r="D14" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B14" s="4" t="s">
+    </row>
+    <row r="15" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="B15" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D14" s="5"/>
-    </row>
-    <row r="15" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="4" t="s">
+      <c r="C15" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="D15" s="5"/>
+    </row>
+    <row r="16" customFormat="false" ht="110.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="B16" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="D15" s="5"/>
-      <c r="E15" s="2" t="s">
+      <c r="C16" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="F15" s="15" t="s">
+      <c r="D16" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E16" s="2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="16" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="4" t="s">
+      <c r="F16" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="B16" s="4" t="s">
+    </row>
+    <row r="17" customFormat="false" ht="66.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="B17" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="D16" s="5"/>
-      <c r="E16" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="F16" s="15" t="s">
+      <c r="C17" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D17" s="5"/>
+      <c r="E17" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F17" s="15" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="50" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E18" s="2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="17" customFormat="false" ht="49.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C17" s="5" t="s">
+      <c r="F18" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="D17" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="F17" s="15" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="D18" s="5" t="s">
+    </row>
+    <row r="19" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="4" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="4" t="s">
+      <c r="B19" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="C19" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="D19" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="D19" s="5"/>
-    </row>
-    <row r="20" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="20" customFormat="false" ht="27.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="4" t="s">
         <v>69</v>
       </c>
@@ -875,116 +914,158 @@
       <c r="C20" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="D20" s="5"/>
-    </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D20" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="D21" s="9" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>75</v>
+      </c>
+      <c r="D21" s="5"/>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>68</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="4" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="D23" s="5"/>
-    </row>
-    <row r="24" customFormat="false" ht="49.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>81</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="4" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="D24" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="E24" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="F24" s="15" t="s">
-        <v>54</v>
-      </c>
+      <c r="D24" s="5"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="B25" s="7" t="s">
+      <c r="B25" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="C25" s="8" t="s">
+      <c r="C25" s="5" t="s">
         <v>87</v>
       </c>
       <c r="D25" s="5" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="26" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="B26" s="12" t="s">
+      <c r="E25" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F25" s="15"/>
+    </row>
+    <row r="26" customFormat="false" ht="40.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="4"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="C26" s="13" t="s">
+      <c r="D26" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="D26" s="5"/>
-      <c r="E26" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="F26" s="15" t="s">
+      <c r="F26" s="15"/>
+    </row>
+    <row r="27" customFormat="false" ht="27.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="4"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="D27" s="5"/>
+      <c r="F27" s="15"/>
+    </row>
+    <row r="28" customFormat="false" ht="27.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="50" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="C29" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E29" s="2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="27" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="D27" s="5"/>
-      <c r="E27" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="F27" s="15" t="s">
+      <c r="F29" s="15" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="50" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="E30" s="2" t="s">
         <v>54</v>
+      </c>
+      <c r="F30" s="15" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated schema in CSV format
</commit_message>
<xml_diff>
--- a/schema/tabular-metajelo.xlsx
+++ b/schema/tabular-metajelo.xlsx
@@ -107,7 +107,7 @@
     <t xml:space="preserve">where to put non-persistent ID (URL + date)?</t>
   </si>
   <si>
-    <t xml:space="preserve">needs own number</t>
+    <t xml:space="preserve">1.5.1.2</t>
   </si>
   <si>
     <t xml:space="preserve">basicMetadata</t>
@@ -122,7 +122,7 @@
     <t xml:space="preserve">Copy from DataCite</t>
   </si>
   <si>
-    <t xml:space="preserve">1.5.1.2</t>
+    <t xml:space="preserve">1.5.1.3</t>
   </si>
   <si>
     <t xml:space="preserve">resourceType</t>
@@ -131,7 +131,7 @@
     <t xml:space="preserve">Description of supplementary product</t>
   </si>
   <si>
-    <t xml:space="preserve">1.5.1.2.1</t>
+    <t xml:space="preserve">1.5.1.3.1</t>
   </si>
   <si>
     <t xml:space="preserve">resourceTypeGeneral</t>
@@ -143,7 +143,7 @@
     <t xml:space="preserve">Controlled vocabulary </t>
   </si>
   <si>
-    <t xml:space="preserve">1.5.1.3</t>
+    <t xml:space="preserve">1.5.1.4</t>
   </si>
   <si>
     <t xml:space="preserve">Format</t>
@@ -155,7 +155,7 @@
     <t xml:space="preserve">optional, repeatable</t>
   </si>
   <si>
-    <t xml:space="preserve">1.5.1.4</t>
+    <t xml:space="preserve">1.5.1.5</t>
   </si>
   <si>
     <t xml:space="preserve">resourceMetadataSource</t>
@@ -167,7 +167,7 @@
     <t xml:space="preserve">optional</t>
   </si>
   <si>
-    <t xml:space="preserve">1.5.1.5</t>
+    <t xml:space="preserve">1.5.1.6</t>
   </si>
   <si>
     <t xml:space="preserve">location</t>
@@ -176,7 +176,7 @@
     <t xml:space="preserve">Wrapper element for metadata describing location of supplementary product</t>
   </si>
   <si>
-    <t xml:space="preserve">1.5.1.5.1</t>
+    <t xml:space="preserve">1.5.1.6.1</t>
   </si>
   <si>
     <t xml:space="preserve">institutionID</t>
@@ -191,7 +191,7 @@
     <t xml:space="preserve">Should this be repeatable? If we have a re3data, a FunderRef, and an OpenAIRE ID?</t>
   </si>
   <si>
-    <t xml:space="preserve">1.5.1.5.2</t>
+    <t xml:space="preserve">1.5.1.6.2</t>
   </si>
   <si>
     <t xml:space="preserve">institutionName</t>
@@ -206,7 +206,7 @@
     <t xml:space="preserve">This should be consistent with re3data schema</t>
   </si>
   <si>
-    <t xml:space="preserve">1.5.1.5.3</t>
+    <t xml:space="preserve">1.5.1.6.3</t>
   </si>
   <si>
     <t xml:space="preserve">institutionType</t>
@@ -218,7 +218,7 @@
     <t xml:space="preserve">Controlled vocabulary based on re3data, possibly expanded</t>
   </si>
   <si>
-    <t xml:space="preserve">1.5.1.5.4</t>
+    <t xml:space="preserve">1.5.1.6.4</t>
   </si>
   <si>
     <t xml:space="preserve">superOrganizationName</t>
@@ -230,7 +230,7 @@
     <t xml:space="preserve">Optional</t>
   </si>
   <si>
-    <t xml:space="preserve">1.5.1.5.5</t>
+    <t xml:space="preserve">1.5.1.6.5</t>
   </si>
   <si>
     <t xml:space="preserve">institutionContact</t>
@@ -242,7 +242,7 @@
     <t xml:space="preserve">Suggested</t>
   </si>
   <si>
-    <t xml:space="preserve">1.5.1.5.6</t>
+    <t xml:space="preserve">1.5.1.6.6</t>
   </si>
   <si>
     <t xml:space="preserve">institutionSustainability</t>
@@ -251,7 +251,7 @@
     <t xml:space="preserve">Wrapper element for assertions concerning institution sustainability</t>
   </si>
   <si>
-    <t xml:space="preserve">1.5.1.5.6.1</t>
+    <t xml:space="preserve">1.5.1.6.6.1</t>
   </si>
   <si>
     <t xml:space="preserve">missionStatementURL</t>
@@ -260,7 +260,7 @@
     <t xml:space="preserve">Link to institution mission statement</t>
   </si>
   <si>
-    <t xml:space="preserve">1.5.1.5.6.2</t>
+    <t xml:space="preserve">1.5.1.6.6.2</t>
   </si>
   <si>
     <t xml:space="preserve">fundingStatementURL</t>
@@ -269,7 +269,7 @@
     <t xml:space="preserve">Link to documentation of institution funding</t>
   </si>
   <si>
-    <t xml:space="preserve">1.5.1.5.7</t>
+    <t xml:space="preserve">1.5.1.6.7</t>
   </si>
   <si>
     <t xml:space="preserve">institutionPolicies</t>
@@ -278,7 +278,7 @@
     <t xml:space="preserve">Wrapper element for set of policies at institution regarding access, archiving, etc)</t>
   </si>
   <si>
-    <t xml:space="preserve">1.5.1.5.7.1</t>
+    <t xml:space="preserve">1.5.1.6.7.1</t>
   </si>
   <si>
     <t xml:space="preserve">institutionPolicy</t>
@@ -299,7 +299,7 @@
     <t xml:space="preserve">Attribute appliesToProduct is true for policies that apply to this product. </t>
   </si>
   <si>
-    <t xml:space="preserve">1.5.1.5.7.1.1</t>
+    <t xml:space="preserve">1.5.1.6.7.1.1</t>
   </si>
   <si>
     <t xml:space="preserve">institutionPolicyFreeText</t>
@@ -311,7 +311,7 @@
     <t xml:space="preserve">Choice</t>
   </si>
   <si>
-    <t xml:space="preserve">1.5.1.5.7.1.2</t>
+    <t xml:space="preserve">1.5.1.6.7.1.2</t>
   </si>
   <si>
     <t xml:space="preserve">institutionPolicyURL</t>
@@ -320,7 +320,7 @@
     <t xml:space="preserve">URI of policy. Attribute re3data:policyURL points to an online copy of the policy. (ID types attribute: DataCite) </t>
   </si>
   <si>
-    <t xml:space="preserve">1.5.1.5.7.2</t>
+    <t xml:space="preserve">1.5.1.6.7.2</t>
   </si>
   <si>
     <t xml:space="preserve">versioning</t>
@@ -339,7 +339,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -372,13 +372,6 @@
       <color rgb="FFCE181E"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FFCE181E"/>
-      <name val="Calibri"/>
-      <family val="1"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -451,7 +444,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -494,10 +487,6 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -595,8 +584,8 @@
   </sheetPr>
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -737,14 +726,14 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="40.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="11" t="s">
+    <row r="10" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="12" t="s">
         <v>30</v>
       </c>
       <c r="D10" s="9" t="s">
@@ -753,7 +742,7 @@
       <c r="E10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F10" s="14" t="s">
+      <c r="F10" s="13" t="s">
         <v>32</v>
       </c>
     </row>
@@ -848,7 +837,7 @@
       <c r="E16" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="F16" s="15" t="s">
+      <c r="F16" s="14" t="s">
         <v>55</v>
       </c>
     </row>
@@ -866,7 +855,7 @@
       <c r="E17" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="F17" s="15" t="s">
+      <c r="F17" s="14" t="s">
         <v>60</v>
       </c>
     </row>
@@ -886,7 +875,7 @@
       <c r="E18" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="F18" s="15" t="s">
+      <c r="F18" s="14" t="s">
         <v>60</v>
       </c>
     </row>
@@ -992,7 +981,7 @@
       <c r="E25" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="F25" s="15"/>
+      <c r="F25" s="14"/>
     </row>
     <row r="26" customFormat="false" ht="40.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="4"/>
@@ -1003,7 +992,7 @@
       <c r="D26" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="F26" s="15"/>
+      <c r="F26" s="14"/>
     </row>
     <row r="27" customFormat="false" ht="27.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="4"/>
@@ -1012,7 +1001,7 @@
         <v>91</v>
       </c>
       <c r="D27" s="5"/>
-      <c r="F27" s="15"/>
+      <c r="F27" s="14"/>
     </row>
     <row r="28" customFormat="false" ht="27.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="4" t="s">
@@ -1032,10 +1021,10 @@
       <c r="A29" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="B29" s="12" t="s">
+      <c r="B29" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="C29" s="13" t="s">
+      <c r="C29" s="12" t="s">
         <v>98</v>
       </c>
       <c r="D29" s="5" t="s">
@@ -1044,7 +1033,7 @@
       <c r="E29" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="F29" s="15" t="s">
+      <c r="F29" s="14" t="s">
         <v>60</v>
       </c>
     </row>
@@ -1064,7 +1053,7 @@
       <c r="E30" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="F30" s="15" t="s">
+      <c r="F30" s="14" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>